<commit_message>
Modified my schedule and added 2 files.
</commit_message>
<xml_diff>
--- a/2018-2019 1st semester.xlsx
+++ b/2018-2019 1st semester.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21001"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1AA38FC-5E4D-4C6B-9645-F1D5122AAF64}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0FFF6AF6-0BD1-4FFB-B5C1-222FBD71E084}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="100">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="322" uniqueCount="104">
   <si>
     <t/>
   </si>
@@ -344,6 +344,37 @@
   </si>
   <si>
     <t>TX1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX3</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>T</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>X1</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>CET4</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>统考</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>监考</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -362,26 +393,13 @@
 TX1--电气16-4
 TX2--电气16-5
 TX3--电气16-6
+WL1--信息16-1
+WL2--信息16-2
 </t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <t>TX3</t>
-    <phoneticPr fontId="7" type="noConversion"/>
-  </si>
-  <si>
-    <r>
-      <t>T</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>X1</t>
-    </r>
+    <t>答疑</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -598,7 +616,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="38">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -624,9 +642,6 @@
     <xf numFmtId="0" fontId="8" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -645,22 +660,13 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -669,10 +675,7 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -696,7 +699,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="3" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -705,10 +708,19 @@
     <xf numFmtId="0" fontId="10" fillId="3" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1029,7 +1041,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="P22" sqref="P22"/>
+      <selection activeCell="R30" sqref="R30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1044,70 +1056,70 @@
     <col min="11" max="11" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="6.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="8.7109375" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="6" customWidth="1"/>
-    <col min="16" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="6" customWidth="1"/>
+    <col min="15" max="19" width="8.7109375" bestFit="1" customWidth="1"/>
     <col min="20" max="22" width="6" customWidth="1"/>
     <col min="23" max="23" width="15.42578125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="26.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="30" t="s">
+      <c r="A1" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="27"/>
-      <c r="I1" s="27"/>
-      <c r="J1" s="27"/>
-      <c r="K1" s="27"/>
-      <c r="L1" s="27"/>
-      <c r="M1" s="27"/>
-      <c r="N1" s="27"/>
-      <c r="O1" s="27"/>
-      <c r="P1" s="27"/>
-      <c r="Q1" s="27"/>
-      <c r="R1" s="27"/>
-      <c r="S1" s="27"/>
-      <c r="T1" s="27"/>
-      <c r="U1" s="27"/>
-      <c r="V1" s="27"/>
-      <c r="W1" s="27"/>
-      <c r="X1" s="27"/>
+      <c r="B1" s="22"/>
+      <c r="C1" s="22"/>
+      <c r="D1" s="22"/>
+      <c r="E1" s="22"/>
+      <c r="F1" s="22"/>
+      <c r="G1" s="22"/>
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="22"/>
+      <c r="N1" s="22"/>
+      <c r="O1" s="22"/>
+      <c r="P1" s="22"/>
+      <c r="Q1" s="22"/>
+      <c r="R1" s="22"/>
+      <c r="S1" s="22"/>
+      <c r="T1" s="22"/>
+      <c r="U1" s="22"/>
+      <c r="V1" s="22"/>
+      <c r="W1" s="22"/>
+      <c r="X1" s="22"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31" t="s">
+      <c r="A2" s="26" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="27"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="27"/>
-      <c r="F2" s="27"/>
-      <c r="G2" s="27"/>
-      <c r="H2" s="27"/>
-      <c r="I2" s="27"/>
-      <c r="J2" s="27"/>
-      <c r="K2" s="27"/>
-      <c r="L2" s="27"/>
-      <c r="M2" s="32" t="s">
+      <c r="B2" s="22"/>
+      <c r="C2" s="22"/>
+      <c r="D2" s="22"/>
+      <c r="E2" s="22"/>
+      <c r="F2" s="22"/>
+      <c r="G2" s="22"/>
+      <c r="H2" s="22"/>
+      <c r="I2" s="22"/>
+      <c r="J2" s="22"/>
+      <c r="K2" s="22"/>
+      <c r="L2" s="22"/>
+      <c r="M2" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="27"/>
-      <c r="O2" s="27"/>
-      <c r="P2" s="27"/>
-      <c r="Q2" s="27"/>
-      <c r="R2" s="27"/>
-      <c r="S2" s="27"/>
-      <c r="T2" s="27"/>
-      <c r="U2" s="27"/>
-      <c r="V2" s="27"/>
-      <c r="W2" s="27"/>
-      <c r="X2" s="27"/>
+      <c r="N2" s="22"/>
+      <c r="O2" s="22"/>
+      <c r="P2" s="22"/>
+      <c r="Q2" s="22"/>
+      <c r="R2" s="22"/>
+      <c r="S2" s="22"/>
+      <c r="T2" s="22"/>
+      <c r="U2" s="22"/>
+      <c r="V2" s="22"/>
+      <c r="W2" s="22"/>
+      <c r="X2" s="22"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1258,43 +1270,43 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="22" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="27" t="s">
+      <c r="D5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="27" t="s">
+      <c r="G5" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="13" t="s">
+      <c r="H5" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="9" t="s">
+      <c r="I5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="12" t="s">
         <v>63</v>
       </c>
       <c r="N5" s="1"/>
@@ -1303,49 +1315,49 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="27" t="s">
+      <c r="T5" s="22" t="s">
         <v>71</v>
       </c>
       <c r="U5" s="1"/>
       <c r="V5" s="1"/>
-      <c r="W5" s="10" t="s">
+      <c r="W5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="X5" s="28" t="s">
-        <v>97</v>
+      <c r="X5" s="23" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="27"/>
+      <c r="A6" s="22"/>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="13" t="s">
+      <c r="D6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="13" t="s">
+      <c r="E6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="9" t="s">
+      <c r="I6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="12" t="s">
         <v>63</v>
       </c>
       <c r="M6" s="1"/>
@@ -1355,52 +1367,52 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="27" t="s">
+      <c r="T6" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
-      <c r="W6" s="10" t="s">
+      <c r="W6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="X6" s="27"/>
+      <c r="X6" s="22"/>
     </row>
     <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="27"/>
+      <c r="A7" s="22"/>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="13" t="s">
+      <c r="D7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" s="9" t="s">
+      <c r="I7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="12" t="s">
         <v>63</v>
       </c>
       <c r="N7" s="1"/>
@@ -1409,28 +1421,30 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="27" t="s">
+      <c r="T7" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U7" s="1"/>
-      <c r="V7" s="1"/>
-      <c r="W7" s="10" t="s">
+      <c r="V7" s="31" t="s">
+        <v>100</v>
+      </c>
+      <c r="W7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="27"/>
+      <c r="X7" s="22"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="27"/>
+      <c r="A8" s="22"/>
       <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="27" t="s">
+      <c r="F8" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="1"/>
@@ -1445,32 +1459,32 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="27" t="s">
+      <c r="T8" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="1"/>
-      <c r="V8" s="1"/>
-      <c r="W8" s="10"/>
-      <c r="X8" s="27"/>
+      <c r="V8" s="32"/>
+      <c r="W8" s="9"/>
+      <c r="X8" s="22"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="27"/>
+      <c r="A9" s="22"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="27" t="s">
+      <c r="F9" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="15"/>
+      <c r="K9" s="14"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1479,32 +1493,32 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="27" t="s">
+      <c r="T9" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
-      <c r="W9" s="10"/>
-      <c r="X9" s="27"/>
+      <c r="W9" s="9"/>
+      <c r="X9" s="22"/>
     </row>
     <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="27"/>
+      <c r="A10" s="22"/>
       <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="27" t="s">
+      <c r="F10" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="15"/>
+      <c r="K10" s="14"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1513,859 +1527,862 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="27" t="s">
+      <c r="T10" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
-      <c r="W10" s="10"/>
-      <c r="X10" s="27"/>
+      <c r="W10" s="9"/>
+      <c r="X10" s="22"/>
     </row>
     <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="27" t="s">
+      <c r="A11" s="22" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C11" s="10"/>
-      <c r="D11" s="10"/>
-      <c r="E11" s="10"/>
-      <c r="F11" s="10"/>
-      <c r="G11" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H11" s="10"/>
-      <c r="I11" s="10"/>
-      <c r="J11" s="10"/>
-      <c r="K11" s="10"/>
-      <c r="L11" s="10"/>
-      <c r="M11" s="10"/>
-      <c r="N11" s="10"/>
-      <c r="O11" s="10"/>
-      <c r="P11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="Q11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="R11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="S11" s="34" t="s">
-        <v>93</v>
-      </c>
-      <c r="T11" s="27" t="s">
+      <c r="C11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H11" s="9"/>
+      <c r="I11" s="9"/>
+      <c r="J11" s="9"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="9"/>
+      <c r="M11" s="9"/>
+      <c r="N11" s="9"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="9"/>
+      <c r="Q11" s="9"/>
+      <c r="R11" s="9"/>
+      <c r="S11" s="9"/>
+      <c r="T11" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
-      <c r="W11" s="10"/>
-      <c r="X11" s="27"/>
+      <c r="W11" s="9"/>
+      <c r="X11" s="22"/>
     </row>
     <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="27"/>
+      <c r="A12" s="22"/>
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="18"/>
-      <c r="G12" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="14" t="s">
+      <c r="D12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="16"/>
+      <c r="G12" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="35"/>
-      <c r="Q12" s="35"/>
-      <c r="R12" s="35"/>
-      <c r="S12" s="35"/>
-      <c r="T12" s="27" t="s">
+      <c r="I12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="9"/>
+      <c r="Q12" s="9"/>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+      <c r="T12" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
-      <c r="W12" s="10" t="s">
+      <c r="W12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="X12" s="27"/>
+      <c r="X12" s="22"/>
     </row>
     <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="27"/>
+      <c r="A13" s="22"/>
       <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C13" s="10"/>
-      <c r="D13" s="10"/>
-      <c r="E13" s="10"/>
-      <c r="F13" s="10"/>
-      <c r="G13" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H13" s="10"/>
-      <c r="I13" s="10"/>
-      <c r="J13" s="10"/>
-      <c r="K13" s="10"/>
-      <c r="L13" s="12" t="s">
+      <c r="C13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H13" s="9"/>
+      <c r="I13" s="9"/>
+      <c r="J13" s="9"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="P13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="S13" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="T13" s="27" t="s">
+      <c r="M13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
-      <c r="W13" s="10" t="s">
+      <c r="W13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="X13" s="27"/>
+      <c r="X13" s="22"/>
     </row>
     <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="27"/>
+      <c r="A14" s="22"/>
       <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="14" t="s">
+      <c r="C14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="14" t="s">
+      <c r="D14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M14" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N14" s="10"/>
-      <c r="O14" s="10"/>
-      <c r="P14" s="10"/>
-      <c r="Q14" s="10"/>
-      <c r="R14" s="10"/>
-      <c r="S14" s="10"/>
-      <c r="T14" s="27" t="s">
+      <c r="I14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N14" s="9"/>
+      <c r="O14" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="P14" s="9"/>
+      <c r="Q14" s="9"/>
+      <c r="R14" s="9"/>
+      <c r="S14" s="9"/>
+      <c r="T14" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
-      <c r="W14" s="10" t="s">
+      <c r="W14" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X14" s="27"/>
+      <c r="X14" s="22"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="27"/>
+      <c r="A15" s="22"/>
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="10"/>
-      <c r="E15" s="29" t="s">
+      <c r="C15" s="9"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="29" t="s">
+      <c r="F15" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="29" t="s">
+      <c r="G15" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="29" t="s">
+      <c r="I15" s="24" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="15"/>
-      <c r="K15" s="33" t="s">
+      <c r="J15" s="14"/>
+      <c r="K15" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="L15" s="19" t="s">
-        <v>98</v>
-      </c>
-      <c r="M15" s="24" t="s">
+      <c r="M15" s="20" t="s">
         <v>87</v>
       </c>
-      <c r="N15" s="10"/>
-      <c r="O15" s="10"/>
-      <c r="P15" s="10"/>
-      <c r="Q15" s="10"/>
-      <c r="R15" s="10"/>
-      <c r="S15" s="10"/>
-      <c r="T15" s="27" t="s">
+      <c r="N15" s="9"/>
+      <c r="O15" s="9"/>
+      <c r="P15" s="9"/>
+      <c r="Q15" s="9"/>
+      <c r="R15" s="9"/>
+      <c r="S15" s="9"/>
+      <c r="T15" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
-      <c r="W15" s="10"/>
-      <c r="X15" s="27"/>
+      <c r="W15" s="9"/>
+      <c r="X15" s="22"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="27"/>
+      <c r="A16" s="22"/>
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
-      <c r="E16" s="23"/>
-      <c r="F16" s="23"/>
-      <c r="G16" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="15"/>
-      <c r="K16" s="25"/>
-      <c r="L16" s="15"/>
-      <c r="M16" s="21"/>
-      <c r="N16" s="10"/>
-      <c r="O16" s="10"/>
-      <c r="P16" s="10"/>
-      <c r="Q16" s="10"/>
-      <c r="R16" s="10"/>
-      <c r="S16" s="10"/>
-      <c r="T16" s="27" t="s">
+      <c r="C16" s="9"/>
+      <c r="D16" s="9"/>
+      <c r="E16" s="19"/>
+      <c r="F16" s="19"/>
+      <c r="G16" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="19"/>
+      <c r="I16" s="19"/>
+      <c r="J16" s="14"/>
+      <c r="K16" s="19"/>
+      <c r="L16" s="14"/>
+      <c r="M16" s="28"/>
+      <c r="N16" s="9"/>
+      <c r="O16" s="9"/>
+      <c r="P16" s="9"/>
+      <c r="Q16" s="9"/>
+      <c r="R16" s="9"/>
+      <c r="S16" s="9"/>
+      <c r="T16" s="22" t="s">
         <v>0</v>
       </c>
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
-      <c r="W16" s="10"/>
-      <c r="X16" s="27"/>
+      <c r="W16" s="9"/>
+      <c r="X16" s="22"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="27" t="s">
+      <c r="A17" s="22" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
-      <c r="F17" s="10"/>
-      <c r="G17" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H17" s="10"/>
-      <c r="I17" s="10"/>
-      <c r="J17" s="10"/>
-      <c r="K17" s="19" t="s">
+      <c r="C17" s="9"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H17" s="9"/>
+      <c r="I17" s="9"/>
+      <c r="J17" s="9"/>
+      <c r="K17" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="19" t="s">
+      <c r="L17" s="12" t="s">
         <v>94</v>
       </c>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="10"/>
-      <c r="P17" s="10"/>
-      <c r="Q17" s="10"/>
-      <c r="R17" s="10"/>
-      <c r="S17" s="10"/>
+      <c r="M17" s="9"/>
+      <c r="N17" s="9"/>
+      <c r="O17" s="9"/>
+      <c r="P17" s="9"/>
+      <c r="Q17" s="9"/>
+      <c r="R17" s="9"/>
+      <c r="S17" s="9"/>
       <c r="T17" s="1"/>
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
-      <c r="W17" s="10"/>
-      <c r="X17" s="27"/>
+      <c r="W17" s="9"/>
+      <c r="X17" s="22"/>
     </row>
     <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="27"/>
+      <c r="A18" s="22"/>
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C18" s="10"/>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
-      <c r="F18" s="10"/>
-      <c r="G18" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10"/>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10"/>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="10"/>
-      <c r="P18" s="10"/>
-      <c r="Q18" s="10"/>
-      <c r="R18" s="10"/>
-      <c r="S18" s="10"/>
+      <c r="C18" s="9"/>
+      <c r="D18" s="9"/>
+      <c r="E18" s="9"/>
+      <c r="F18" s="9"/>
+      <c r="G18" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H18" s="9"/>
+      <c r="I18" s="9"/>
+      <c r="J18" s="9"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="9"/>
+      <c r="M18" s="9"/>
+      <c r="N18" s="9"/>
+      <c r="O18" s="9"/>
+      <c r="P18" s="9"/>
+      <c r="Q18" s="9"/>
+      <c r="R18" s="9"/>
+      <c r="S18" s="9"/>
       <c r="T18" s="1"/>
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
-      <c r="W18" s="10"/>
-      <c r="X18" s="27"/>
+      <c r="W18" s="9"/>
+      <c r="X18" s="22"/>
     </row>
     <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="27"/>
+      <c r="A19" s="22"/>
       <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="10"/>
-      <c r="E19" s="10"/>
-      <c r="F19" s="10"/>
-      <c r="G19" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H19" s="10"/>
-      <c r="I19" s="10"/>
-      <c r="J19" s="36" t="s">
+      <c r="C19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H19" s="9"/>
+      <c r="I19" s="9"/>
+      <c r="J19" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="K19" s="34" t="s">
+      <c r="K19" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="34" t="s">
+      <c r="L19" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="M19" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="N19" s="34" t="s">
+      <c r="M19" s="9"/>
+      <c r="N19" s="33" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="P19" s="34" t="s">
-        <v>91</v>
-      </c>
-      <c r="Q19" s="34" t="s">
-        <v>92</v>
-      </c>
-      <c r="R19" s="10"/>
-      <c r="S19" s="10"/>
+      <c r="O19" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="P19" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q19" s="9"/>
+      <c r="R19" s="9"/>
+      <c r="S19" s="9"/>
       <c r="T19" s="1"/>
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
-      <c r="W19" s="10"/>
-      <c r="X19" s="27"/>
+      <c r="W19" s="9"/>
+      <c r="X19" s="22"/>
     </row>
     <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="27"/>
+      <c r="A20" s="22"/>
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C20" s="10"/>
-      <c r="D20" s="10"/>
-      <c r="E20" s="10"/>
-      <c r="F20" s="10"/>
-      <c r="G20" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H20" s="10"/>
-      <c r="I20" s="10"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="35"/>
-      <c r="L20" s="35"/>
-      <c r="M20" s="35"/>
-      <c r="N20" s="35"/>
-      <c r="O20" s="35"/>
-      <c r="P20" s="35"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="10"/>
-      <c r="S20" s="10"/>
+      <c r="C20" s="9"/>
+      <c r="D20" s="9"/>
+      <c r="E20" s="9"/>
+      <c r="F20" s="9"/>
+      <c r="G20" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H20" s="9"/>
+      <c r="I20" s="9"/>
+      <c r="J20" s="34"/>
+      <c r="K20" s="34"/>
+      <c r="L20" s="34"/>
+      <c r="M20" s="9"/>
+      <c r="N20" s="34"/>
+      <c r="O20" s="30"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="9"/>
+      <c r="R20" s="9"/>
+      <c r="S20" s="9"/>
       <c r="T20" s="1"/>
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
-      <c r="W20" s="10"/>
-      <c r="X20" s="27"/>
+      <c r="W20" s="9"/>
+      <c r="X20" s="22"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="27"/>
+      <c r="A21" s="22"/>
       <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C21" s="10"/>
-      <c r="D21" s="10"/>
-      <c r="E21" s="10"/>
-      <c r="F21" s="10"/>
-      <c r="G21" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H21" s="10"/>
-      <c r="I21" s="10"/>
-      <c r="J21" s="10"/>
-      <c r="K21" s="19" t="s">
-        <v>99</v>
-      </c>
-      <c r="L21" s="19" t="s">
+      <c r="C21" s="9"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H21" s="9"/>
+      <c r="I21" s="9"/>
+      <c r="J21" s="9"/>
+      <c r="K21" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="L21" s="12" t="s">
         <v>96</v>
       </c>
-      <c r="M21" s="10"/>
-      <c r="N21" s="10"/>
-      <c r="O21" s="10"/>
-      <c r="P21" s="10"/>
-      <c r="Q21" s="10"/>
-      <c r="R21" s="10"/>
-      <c r="S21" s="10"/>
+      <c r="M21" s="9"/>
+      <c r="N21" s="9"/>
+      <c r="O21" s="17" t="s">
+        <v>103</v>
+      </c>
+      <c r="P21" s="9"/>
+      <c r="Q21" s="9"/>
+      <c r="R21" s="9"/>
+      <c r="S21" s="9"/>
       <c r="T21" s="1"/>
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
-      <c r="W21" s="10"/>
-      <c r="X21" s="27"/>
+      <c r="W21" s="9"/>
+      <c r="X21" s="22"/>
     </row>
     <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="27"/>
+      <c r="A22" s="22"/>
       <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C22" s="10"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="10"/>
-      <c r="K22" s="10"/>
-      <c r="L22" s="10"/>
-      <c r="M22" s="10"/>
-      <c r="N22" s="10"/>
-      <c r="O22" s="10"/>
-      <c r="P22" s="10"/>
-      <c r="Q22" s="10"/>
-      <c r="R22" s="10"/>
-      <c r="S22" s="10"/>
+      <c r="C22" s="9"/>
+      <c r="D22" s="9"/>
+      <c r="E22" s="9"/>
+      <c r="F22" s="9"/>
+      <c r="G22" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H22" s="9"/>
+      <c r="I22" s="9"/>
+      <c r="J22" s="9"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="9"/>
+      <c r="M22" s="9"/>
+      <c r="N22" s="9"/>
+      <c r="O22" s="9"/>
+      <c r="P22" s="9"/>
+      <c r="Q22" s="9"/>
+      <c r="R22" s="9"/>
+      <c r="S22" s="9"/>
       <c r="T22" s="1"/>
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
-      <c r="W22" s="10"/>
-      <c r="X22" s="27"/>
+      <c r="W22" s="9"/>
+      <c r="X22" s="22"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="27" t="s">
+      <c r="A23" s="22" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C23" s="10"/>
-      <c r="D23" s="10"/>
-      <c r="E23" s="10"/>
-      <c r="F23" s="10"/>
-      <c r="G23" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H23" s="10"/>
-      <c r="I23" s="10"/>
-      <c r="J23" s="10"/>
-      <c r="K23" s="10"/>
-      <c r="L23" s="10"/>
-      <c r="M23" s="10"/>
-      <c r="N23" s="10"/>
-      <c r="O23" s="10"/>
-      <c r="P23" s="10"/>
-      <c r="Q23" s="10"/>
-      <c r="R23" s="10"/>
-      <c r="S23" s="10"/>
+      <c r="C23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H23" s="9"/>
+      <c r="I23" s="9"/>
+      <c r="J23" s="9"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="9"/>
+      <c r="M23" s="9"/>
+      <c r="N23" s="9"/>
+      <c r="O23" s="9"/>
+      <c r="P23" s="9"/>
+      <c r="Q23" s="9"/>
+      <c r="R23" s="9"/>
+      <c r="S23" s="9"/>
       <c r="T23" s="1"/>
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
-      <c r="W23" s="10"/>
-      <c r="X23" s="27"/>
+      <c r="W23" s="9"/>
+      <c r="X23" s="22"/>
     </row>
     <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="27"/>
+      <c r="A24" s="22"/>
       <c r="B24" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C24" s="10"/>
-      <c r="D24" s="10"/>
-      <c r="E24" s="10"/>
-      <c r="F24" s="10"/>
-      <c r="G24" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H24" s="10"/>
-      <c r="I24" s="10"/>
-      <c r="J24" s="10"/>
-      <c r="K24" s="10"/>
-      <c r="L24" s="10"/>
-      <c r="M24" s="10"/>
-      <c r="N24" s="10"/>
-      <c r="O24" s="10"/>
-      <c r="P24" s="10"/>
-      <c r="Q24" s="10"/>
-      <c r="R24" s="10"/>
-      <c r="S24" s="10"/>
-      <c r="T24" s="11"/>
+      <c r="C24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="9"/>
+      <c r="F24" s="9"/>
+      <c r="G24" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H24" s="9"/>
+      <c r="I24" s="9"/>
+      <c r="J24" s="9"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="9"/>
+      <c r="M24" s="9"/>
+      <c r="N24" s="9"/>
+      <c r="O24" s="9"/>
+      <c r="P24" s="9"/>
+      <c r="Q24" s="9"/>
+      <c r="R24" s="9"/>
+      <c r="S24" s="9"/>
+      <c r="T24" s="10"/>
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
-      <c r="W24" s="10"/>
-      <c r="X24" s="27"/>
+      <c r="W24" s="9"/>
+      <c r="X24" s="22"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="27"/>
+      <c r="A25" s="22"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="14" t="s">
+      <c r="C25" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="14" t="s">
+      <c r="D25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="13" t="s">
         <v>67</v>
       </c>
-      <c r="I25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="10"/>
-      <c r="N25" s="10"/>
-      <c r="O25" s="10"/>
-      <c r="P25" s="10"/>
-      <c r="Q25" s="10"/>
-      <c r="R25" s="10"/>
-      <c r="S25" s="10"/>
+      <c r="I25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="N25" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="O25" s="29" t="s">
+        <v>92</v>
+      </c>
+      <c r="P25" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="Q25" s="9"/>
+      <c r="R25" s="9"/>
+      <c r="S25" s="9"/>
       <c r="T25" s="1"/>
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
-      <c r="W25" s="10" t="s">
+      <c r="W25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X25" s="27"/>
+      <c r="X25" s="22"/>
     </row>
     <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="27"/>
+      <c r="A26" s="22"/>
       <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="14" t="s">
+      <c r="C26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="14" t="s">
+      <c r="D26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L26" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M26" s="10"/>
-      <c r="N26" s="10"/>
-      <c r="O26" s="10"/>
-      <c r="P26" s="10"/>
-      <c r="Q26" s="10"/>
-      <c r="R26" s="10"/>
-      <c r="S26" s="10"/>
+      <c r="I26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" s="34"/>
+      <c r="N26" s="30"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="9"/>
+      <c r="R26" s="9"/>
+      <c r="S26" s="9"/>
       <c r="T26" s="1"/>
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
-      <c r="W26" s="10" t="s">
+      <c r="W26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="X26" s="27"/>
+      <c r="X26" s="22"/>
     </row>
     <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="27"/>
+      <c r="A27" s="22"/>
       <c r="B27" s="1" t="s">
         <v>54</v>
       </c>
-      <c r="C27" s="10"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="22" t="s">
+      <c r="C27" s="9"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="22" t="s">
+      <c r="F27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="22" t="s">
+      <c r="G27" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="18" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="22" t="s">
+      <c r="I27" s="18" t="s">
         <v>89</v>
       </c>
-      <c r="J27" s="10"/>
-      <c r="K27" s="24" t="s">
+      <c r="J27" s="9"/>
+      <c r="K27" s="20" t="s">
         <v>90</v>
       </c>
-      <c r="L27" s="16"/>
-      <c r="M27" s="20" t="s">
+      <c r="L27" s="12" t="s">
+        <v>97</v>
+      </c>
+      <c r="M27" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="N27" s="10"/>
-      <c r="O27" s="10"/>
-      <c r="P27" s="10"/>
-      <c r="Q27" s="10"/>
-      <c r="R27" s="10"/>
-      <c r="S27" s="10"/>
+      <c r="N27" s="9"/>
+      <c r="O27" s="9"/>
+      <c r="P27" s="9"/>
+      <c r="Q27" s="9"/>
+      <c r="R27" s="9"/>
+      <c r="S27" s="9"/>
       <c r="T27" s="1"/>
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
-      <c r="W27" s="10"/>
-      <c r="X27" s="27"/>
+      <c r="W27" s="9"/>
+      <c r="X27" s="22"/>
     </row>
     <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="27"/>
+      <c r="A28" s="22"/>
       <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C28" s="10"/>
-      <c r="D28" s="10"/>
-      <c r="E28" s="23"/>
-      <c r="F28" s="23"/>
-      <c r="G28" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="10"/>
-      <c r="K28" s="25"/>
-      <c r="L28" s="17"/>
-      <c r="M28" s="21"/>
-      <c r="N28" s="10"/>
-      <c r="O28" s="10"/>
-      <c r="P28" s="10"/>
-      <c r="Q28" s="10"/>
-      <c r="R28" s="10"/>
-      <c r="S28" s="10"/>
+      <c r="C28" s="9"/>
+      <c r="D28" s="9"/>
+      <c r="E28" s="19"/>
+      <c r="F28" s="19"/>
+      <c r="G28" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="19"/>
+      <c r="I28" s="19"/>
+      <c r="J28" s="9"/>
+      <c r="K28" s="19"/>
+      <c r="L28" s="15"/>
+      <c r="M28" s="28"/>
+      <c r="N28" s="9"/>
+      <c r="O28" s="9"/>
+      <c r="P28" s="9"/>
+      <c r="Q28" s="9"/>
+      <c r="R28" s="9"/>
+      <c r="S28" s="9"/>
       <c r="T28" s="1"/>
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
-      <c r="W28" s="10"/>
-      <c r="X28" s="27"/>
+      <c r="W28" s="9"/>
+      <c r="X28" s="22"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="27" t="s">
+      <c r="A29" s="22" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C29" s="10"/>
-      <c r="D29" s="10"/>
-      <c r="E29" s="10"/>
-      <c r="F29" s="14" t="s">
+      <c r="C29" s="9"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10"/>
-      <c r="J29" s="10"/>
-      <c r="K29" s="19" t="s">
+      <c r="G29" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9"/>
+      <c r="K29" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="L29" s="10"/>
-      <c r="M29" s="10"/>
-      <c r="N29" s="10"/>
-      <c r="O29" s="10"/>
-      <c r="P29" s="10"/>
-      <c r="Q29" s="10"/>
-      <c r="R29" s="10"/>
-      <c r="S29" s="10"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="9"/>
+      <c r="N29" s="9"/>
+      <c r="O29" s="9"/>
+      <c r="P29" s="9"/>
+      <c r="Q29" s="9"/>
+      <c r="R29" s="9"/>
+      <c r="S29" s="9"/>
       <c r="T29" s="1"/>
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
-      <c r="W29" s="10"/>
-      <c r="X29" s="27"/>
+      <c r="W29" s="9"/>
+      <c r="X29" s="22"/>
     </row>
     <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="27"/>
+      <c r="A30" s="22"/>
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C30" s="10"/>
-      <c r="D30" s="10"/>
-      <c r="E30" s="10"/>
-      <c r="G30" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10"/>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="12" t="s">
+      <c r="C30" s="9"/>
+      <c r="D30" s="9"/>
+      <c r="E30" s="9"/>
+      <c r="G30" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="13" t="s">
         <v>66</v>
       </c>
-      <c r="M30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="N30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="O30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="P30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="S30" s="12" t="s">
+      <c r="M30" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="S30" s="11" t="s">
         <v>63</v>
       </c>
       <c r="T30" s="1"/>
       <c r="U30" s="1"/>
       <c r="V30" s="1"/>
-      <c r="W30" s="10" t="s">
+      <c r="W30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="X30" s="27"/>
+      <c r="X30" s="22"/>
     </row>
     <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="27"/>
+      <c r="A31" s="22"/>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C31" s="10"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="14" t="s">
+      <c r="C31" s="9"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="27" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="14" t="s">
+      <c r="F31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="22" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="13" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L31" s="10"/>
-      <c r="M31" s="10"/>
-      <c r="N31" s="10"/>
-      <c r="O31" s="10"/>
-      <c r="P31" s="10"/>
-      <c r="Q31" s="10"/>
-      <c r="R31" s="10"/>
-      <c r="S31" s="10"/>
+      <c r="I31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="L31" s="9"/>
+      <c r="M31" s="9"/>
+      <c r="N31" s="29" t="s">
+        <v>91</v>
+      </c>
+      <c r="O31" s="29" t="s">
+        <v>93</v>
+      </c>
+      <c r="P31" s="9"/>
+      <c r="Q31" s="9"/>
+      <c r="R31" s="9"/>
+      <c r="S31" s="9"/>
       <c r="T31" s="1"/>
       <c r="U31" s="1"/>
       <c r="V31" s="1"/>
-      <c r="W31" s="10" t="s">
+      <c r="W31" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="X31" s="27"/>
+      <c r="X31" s="22"/>
     </row>
     <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="27"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -2373,7 +2390,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="27" t="s">
+      <c r="G32" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H32" s="1"/>
@@ -2381,9 +2398,11 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="1"/>
-      <c r="N32" s="1"/>
-      <c r="O32" s="1"/>
+      <c r="M32" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="N32" s="30"/>
+      <c r="O32" s="30"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
@@ -2392,10 +2411,10 @@
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
-      <c r="X32" s="27"/>
+      <c r="X32" s="22"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="27"/>
+      <c r="A33" s="22"/>
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2403,7 +2422,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="27" t="s">
+      <c r="G33" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H33" s="1"/>
@@ -2413,7 +2432,9 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="1"/>
+      <c r="O33" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="P33" s="1"/>
       <c r="Q33" s="1"/>
       <c r="R33" s="1"/>
@@ -2422,10 +2443,10 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="27"/>
+      <c r="X33" s="22"/>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="27"/>
+      <c r="A34" s="22"/>
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
@@ -2433,7 +2454,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="27" t="s">
+      <c r="G34" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H34" s="1"/>
@@ -2452,10 +2473,10 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="27"/>
+      <c r="X34" s="22"/>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="27" t="s">
+      <c r="A35" s="22" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2463,16 +2484,16 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="27" t="s">
+      <c r="E35" s="22" t="s">
         <v>70</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="27" t="s">
+      <c r="G35" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="27" t="s">
+      <c r="J35" s="22" t="s">
         <v>68</v>
       </c>
       <c r="K35" s="1"/>
@@ -2481,32 +2502,34 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="1"/>
+      <c r="Q35" s="31" t="s">
+        <v>99</v>
+      </c>
       <c r="R35" s="1"/>
       <c r="S35" s="1"/>
       <c r="T35" s="1"/>
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="27"/>
+      <c r="X35" s="22"/>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="27"/>
+      <c r="A36" s="22"/>
       <c r="B36" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="27" t="s">
+      <c r="E36" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="27" t="s">
+      <c r="G36" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="27" t="s">
+      <c r="J36" s="22" t="s">
         <v>0</v>
       </c>
       <c r="K36" s="1"/>
@@ -2515,32 +2538,32 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="1"/>
+      <c r="Q36" s="32"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="27"/>
+      <c r="X36" s="22"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="27"/>
+      <c r="A37" s="22"/>
       <c r="B37" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="27" t="s">
+      <c r="E37" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="27" t="s">
+      <c r="G37" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="27" t="s">
+      <c r="J37" s="22" t="s">
         <v>0</v>
       </c>
       <c r="K37" s="1"/>
@@ -2556,25 +2579,25 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="27"/>
+      <c r="X37" s="22"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="27"/>
+      <c r="A38" s="22"/>
       <c r="B38" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="27" t="s">
+      <c r="E38" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="27" t="s">
+      <c r="G38" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="27" t="s">
+      <c r="J38" s="22" t="s">
         <v>0</v>
       </c>
       <c r="K38" s="1"/>
@@ -2590,25 +2613,25 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="27"/>
+      <c r="X38" s="22"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="27"/>
+      <c r="A39" s="22"/>
       <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="27" t="s">
+      <c r="E39" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="27" t="s">
+      <c r="G39" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="27" t="s">
+      <c r="J39" s="22" t="s">
         <v>0</v>
       </c>
       <c r="K39" s="1"/>
@@ -2624,25 +2647,25 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="27"/>
+      <c r="X39" s="22"/>
     </row>
     <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="27"/>
+      <c r="A40" s="22"/>
       <c r="B40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="27" t="s">
+      <c r="E40" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="27" t="s">
+      <c r="G40" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="27" t="s">
+      <c r="J40" s="22" t="s">
         <v>0</v>
       </c>
       <c r="K40" s="1"/>
@@ -2658,10 +2681,10 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="27"/>
+      <c r="X40" s="22"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="27" t="s">
+      <c r="A41" s="22" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2669,11 +2692,11 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="27" t="s">
+      <c r="E41" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="27" t="s">
+      <c r="G41" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H41" s="1"/>
@@ -2687,7 +2710,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="27" t="s">
+      <c r="S41" s="22" t="s">
         <v>71</v>
       </c>
       <c r="T41" s="1"/>
@@ -2696,20 +2719,20 @@
       <c r="W41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="X41" s="27"/>
+      <c r="X41" s="22"/>
     </row>
     <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="27"/>
+      <c r="A42" s="22"/>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="27" t="s">
+      <c r="E42" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="1"/>
-      <c r="G42" s="27" t="s">
+      <c r="G42" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H42" s="1"/>
@@ -2723,7 +2746,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="27" t="s">
+      <c r="S42" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T42" s="1"/>
@@ -2732,20 +2755,20 @@
       <c r="W42" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="X42" s="27"/>
+      <c r="X42" s="22"/>
     </row>
     <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="27"/>
+      <c r="A43" s="22"/>
       <c r="B43" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="27" t="s">
+      <c r="E43" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="27" t="s">
+      <c r="G43" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H43" s="1"/>
@@ -2759,7 +2782,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="27" t="s">
+      <c r="S43" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T43" s="1"/>
@@ -2768,20 +2791,20 @@
       <c r="W43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="X43" s="27"/>
+      <c r="X43" s="22"/>
     </row>
     <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="27"/>
+      <c r="A44" s="22"/>
       <c r="B44" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="27" t="s">
+      <c r="E44" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="1"/>
-      <c r="G44" s="27" t="s">
+      <c r="G44" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H44" s="1"/>
@@ -2795,7 +2818,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="27" t="s">
+      <c r="S44" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T44" s="1"/>
@@ -2804,20 +2827,20 @@
       <c r="W44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="X44" s="27"/>
+      <c r="X44" s="22"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="27"/>
+      <c r="A45" s="22"/>
       <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="27" t="s">
+      <c r="E45" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="1"/>
-      <c r="G45" s="27" t="s">
+      <c r="G45" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H45" s="1"/>
@@ -2831,7 +2854,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="27" t="s">
+      <c r="S45" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T45" s="1"/>
@@ -2840,20 +2863,20 @@
       <c r="W45" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="X45" s="27"/>
+      <c r="X45" s="22"/>
     </row>
     <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="27"/>
+      <c r="A46" s="22"/>
       <c r="B46" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="27" t="s">
+      <c r="E46" s="22" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="1"/>
-      <c r="G46" s="27" t="s">
+      <c r="G46" s="22" t="s">
         <v>0</v>
       </c>
       <c r="H46" s="1"/>
@@ -2867,53 +2890,60 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="27" t="s">
+      <c r="S46" s="22" t="s">
         <v>0</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="27"/>
+      <c r="X46" s="22"/>
     </row>
     <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="26" t="s">
+      <c r="A47" s="21" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="27"/>
-      <c r="C47" s="27"/>
-      <c r="D47" s="27"/>
-      <c r="E47" s="27"/>
-      <c r="F47" s="27"/>
-      <c r="G47" s="27"/>
-      <c r="H47" s="27"/>
-      <c r="I47" s="27"/>
-      <c r="J47" s="27"/>
-      <c r="K47" s="27"/>
-      <c r="L47" s="27"/>
-      <c r="M47" s="27"/>
-      <c r="N47" s="27"/>
-      <c r="O47" s="27"/>
-      <c r="P47" s="27"/>
-      <c r="Q47" s="27"/>
-      <c r="R47" s="27"/>
-      <c r="S47" s="27"/>
-      <c r="T47" s="27"/>
-      <c r="U47" s="27"/>
-      <c r="V47" s="27"/>
-      <c r="W47" s="27"/>
-      <c r="X47" s="27"/>
+      <c r="B47" s="22"/>
+      <c r="C47" s="22"/>
+      <c r="D47" s="22"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="22"/>
+      <c r="G47" s="22"/>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22"/>
+      <c r="J47" s="22"/>
+      <c r="K47" s="22"/>
+      <c r="L47" s="22"/>
+      <c r="M47" s="22"/>
+      <c r="N47" s="22"/>
+      <c r="O47" s="22"/>
+      <c r="P47" s="22"/>
+      <c r="Q47" s="22"/>
+      <c r="R47" s="22"/>
+      <c r="S47" s="22"/>
+      <c r="T47" s="22"/>
+      <c r="U47" s="22"/>
+      <c r="V47" s="22"/>
+      <c r="W47" s="22"/>
+      <c r="X47" s="22"/>
     </row>
   </sheetData>
-  <mergeCells count="42">
-    <mergeCell ref="O19:O20"/>
+  <mergeCells count="44">
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="O25:O26"/>
     <mergeCell ref="J19:J20"/>
     <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="O31:O32"/>
     <mergeCell ref="P19:P20"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M19:M20"/>
-    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="P25:P26"/>
     <mergeCell ref="A1:X1"/>
     <mergeCell ref="A2:L2"/>
     <mergeCell ref="M2:X2"/>
@@ -2922,10 +2952,6 @@
     <mergeCell ref="I15:I16"/>
     <mergeCell ref="K15:K16"/>
     <mergeCell ref="M15:M16"/>
-    <mergeCell ref="P11:P12"/>
-    <mergeCell ref="Q11:Q12"/>
-    <mergeCell ref="S11:S12"/>
-    <mergeCell ref="R11:R12"/>
     <mergeCell ref="A47:X47"/>
     <mergeCell ref="X5:X46"/>
     <mergeCell ref="J35:J40"/>
@@ -2942,7 +2968,6 @@
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="M27:M28"/>
     <mergeCell ref="E27:E28"/>
     <mergeCell ref="F27:F28"/>
     <mergeCell ref="H27:H28"/>

</xml_diff>

<commit_message>
Modified my schedule and added some files.
</commit_message>
<xml_diff>
--- a/2018-2019 1st semester.xlsx
+++ b/2018-2019 1st semester.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Administrator\Desktop\MySchedule\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EE1FF13-B4F1-4E13-B472-D6BC5B6E048E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B66C243-9108-4D55-90D9-0223285EC5B5}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12135" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="966" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="652" uniqueCount="108">
   <si>
     <t/>
   </si>
@@ -375,6 +375,33 @@
   </si>
   <si>
     <t>监考</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <r>
+      <t>J</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <rFont val="宋体"/>
+        <family val="3"/>
+        <charset val="134"/>
+      </rPr>
+      <t>S</t>
+    </r>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZZ1</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZZ2</t>
+    <phoneticPr fontId="7" type="noConversion"/>
+  </si>
+  <si>
+    <t>SZZ3</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
@@ -395,22 +422,14 @@
 TX3--电气16-6
 WL1--信息16-1
 WL2--信息16-2
+SZZ1--电气16-3、4
+SZZ2--电气16-2
+SZZ3--电气16-5、6
 </t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
   <si>
-    <r>
-      <t>J</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="宋体"/>
-        <family val="3"/>
-        <charset val="134"/>
-      </rPr>
-      <t>S</t>
-    </r>
+    <t>监考</t>
     <phoneticPr fontId="7" type="noConversion"/>
   </si>
 </sst>
@@ -627,7 +646,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -659,9 +678,6 @@
     <xf numFmtId="0" fontId="2" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -677,61 +693,67 @@
     <xf numFmtId="0" fontId="8" fillId="7" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="6" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1052,7 +1074,7 @@
   <dimension ref="A1:X47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19:R20"/>
+      <selection activeCell="U23" sqref="U23:U28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1075,62 +1097,62 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:24" ht="32.450000000000003" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="25" t="s">
+      <c r="A1" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="21"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-      <c r="T1" s="21"/>
-      <c r="U1" s="21"/>
-      <c r="V1" s="21"/>
-      <c r="W1" s="21"/>
-      <c r="X1" s="21"/>
+      <c r="B1" s="29"/>
+      <c r="C1" s="29"/>
+      <c r="D1" s="29"/>
+      <c r="E1" s="29"/>
+      <c r="F1" s="29"/>
+      <c r="G1" s="29"/>
+      <c r="H1" s="29"/>
+      <c r="I1" s="29"/>
+      <c r="J1" s="29"/>
+      <c r="K1" s="29"/>
+      <c r="L1" s="29"/>
+      <c r="M1" s="29"/>
+      <c r="N1" s="29"/>
+      <c r="O1" s="29"/>
+      <c r="P1" s="29"/>
+      <c r="Q1" s="29"/>
+      <c r="R1" s="29"/>
+      <c r="S1" s="29"/>
+      <c r="T1" s="29"/>
+      <c r="U1" s="29"/>
+      <c r="V1" s="29"/>
+      <c r="W1" s="29"/>
+      <c r="X1" s="29"/>
     </row>
     <row r="2" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="26" t="s">
+      <c r="A2" s="30" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="21"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="27" t="s">
+      <c r="B2" s="29"/>
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="29"/>
+      <c r="F2" s="29"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="29"/>
+      <c r="I2" s="29"/>
+      <c r="J2" s="29"/>
+      <c r="K2" s="29"/>
+      <c r="L2" s="29"/>
+      <c r="M2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="21"/>
-      <c r="Q2" s="21"/>
-      <c r="R2" s="21"/>
-      <c r="S2" s="21"/>
-      <c r="T2" s="21"/>
-      <c r="U2" s="21"/>
-      <c r="V2" s="21"/>
-      <c r="W2" s="21"/>
-      <c r="X2" s="21"/>
+      <c r="N2" s="29"/>
+      <c r="O2" s="29"/>
+      <c r="P2" s="29"/>
+      <c r="Q2" s="29"/>
+      <c r="R2" s="29"/>
+      <c r="S2" s="29"/>
+      <c r="T2" s="29"/>
+      <c r="U2" s="29"/>
+      <c r="V2" s="29"/>
+      <c r="W2" s="29"/>
+      <c r="X2" s="29"/>
     </row>
     <row r="3" spans="1:24" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1281,43 +1303,43 @@
       </c>
     </row>
     <row r="5" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21" t="s">
+      <c r="A5" s="29" t="s">
         <v>49</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="D5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F5" s="21" t="s">
+      <c r="D5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F5" s="29" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="21" t="s">
+      <c r="G5" s="29" t="s">
         <v>69</v>
       </c>
-      <c r="H5" s="12" t="s">
+      <c r="H5" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="I5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L5" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M5" s="12" t="s">
+      <c r="I5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L5" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M5" s="11" t="s">
         <v>63</v>
       </c>
       <c r="N5" s="1"/>
@@ -1326,7 +1348,7 @@
       <c r="Q5" s="1"/>
       <c r="R5" s="1"/>
       <c r="S5" s="1"/>
-      <c r="T5" s="21" t="s">
+      <c r="T5" s="29" t="s">
         <v>71</v>
       </c>
       <c r="U5" s="1"/>
@@ -1334,41 +1356,41 @@
       <c r="W5" s="9" t="s">
         <v>72</v>
       </c>
-      <c r="X5" s="22" t="s">
-        <v>102</v>
+      <c r="X5" s="34" t="s">
+        <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
+      <c r="A6" s="29"/>
       <c r="B6" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C6" s="1"/>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="E6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G6" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H6" s="12" t="s">
+      <c r="E6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G6" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H6" s="11" t="s">
         <v>65</v>
       </c>
-      <c r="I6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K6" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L6" s="12" t="s">
+      <c r="I6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K6" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L6" s="11" t="s">
         <v>63</v>
       </c>
       <c r="M6" s="1"/>
@@ -1378,7 +1400,7 @@
       <c r="Q6" s="1"/>
       <c r="R6" s="1"/>
       <c r="S6" s="1"/>
-      <c r="T6" s="21" t="s">
+      <c r="T6" s="29" t="s">
         <v>0</v>
       </c>
       <c r="U6" s="1"/>
@@ -1386,44 +1408,44 @@
       <c r="W6" s="9" t="s">
         <v>74</v>
       </c>
-      <c r="X6" s="21"/>
+      <c r="X6" s="29"/>
     </row>
     <row r="7" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21"/>
+      <c r="A7" s="29"/>
       <c r="B7" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="E7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G7" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H7" s="12" t="s">
+      <c r="D7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="E7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="F7" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G7" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H7" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="I7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="J7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="K7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="L7" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="M7" s="12" t="s">
+      <c r="I7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="J7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="K7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="L7" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="M7" s="11" t="s">
         <v>63</v>
       </c>
       <c r="N7" s="1"/>
@@ -1432,30 +1454,30 @@
       <c r="Q7" s="1"/>
       <c r="R7" s="1"/>
       <c r="S7" s="1"/>
-      <c r="T7" s="21" t="s">
+      <c r="T7" s="29" t="s">
         <v>0</v>
       </c>
       <c r="U7" s="1"/>
-      <c r="V7" s="31" t="s">
+      <c r="V7" s="21" t="s">
         <v>100</v>
       </c>
       <c r="W7" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X7" s="21"/>
+      <c r="X7" s="29"/>
     </row>
     <row r="8" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
+      <c r="A8" s="29"/>
       <c r="B8" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C8" s="1"/>
       <c r="D8" s="1"/>
       <c r="E8" s="1"/>
-      <c r="F8" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G8" s="21" t="s">
+      <c r="F8" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H8" s="1"/>
@@ -1470,32 +1492,32 @@
       <c r="Q8" s="1"/>
       <c r="R8" s="1"/>
       <c r="S8" s="1"/>
-      <c r="T8" s="21" t="s">
+      <c r="T8" s="29" t="s">
         <v>0</v>
       </c>
       <c r="U8" s="1"/>
-      <c r="V8" s="32"/>
+      <c r="V8" s="22"/>
       <c r="W8" s="9"/>
-      <c r="X8" s="21"/>
+      <c r="X8" s="29"/>
     </row>
     <row r="9" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
+      <c r="A9" s="29"/>
       <c r="B9" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C9" s="1"/>
       <c r="D9" s="1"/>
       <c r="E9" s="1"/>
-      <c r="F9" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G9" s="21" t="s">
+      <c r="F9" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H9" s="1"/>
       <c r="I9" s="1"/>
       <c r="J9" s="1"/>
-      <c r="K9" s="14"/>
+      <c r="K9" s="13"/>
       <c r="L9" s="1"/>
       <c r="M9" s="1"/>
       <c r="N9" s="1"/>
@@ -1504,32 +1526,32 @@
       <c r="Q9" s="1"/>
       <c r="R9" s="1"/>
       <c r="S9" s="1"/>
-      <c r="T9" s="21" t="s">
+      <c r="T9" s="29" t="s">
         <v>0</v>
       </c>
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
       <c r="W9" s="9"/>
-      <c r="X9" s="21"/>
+      <c r="X9" s="29"/>
     </row>
     <row r="10" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21"/>
+      <c r="A10" s="29"/>
       <c r="B10" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-      <c r="F10" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="G10" s="21" t="s">
+      <c r="F10" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="G10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H10" s="1"/>
       <c r="I10" s="1"/>
       <c r="J10" s="1"/>
-      <c r="K10" s="14"/>
+      <c r="K10" s="13"/>
       <c r="L10" s="1"/>
       <c r="M10" s="1"/>
       <c r="N10" s="1"/>
@@ -1538,16 +1560,16 @@
       <c r="Q10" s="1"/>
       <c r="R10" s="1"/>
       <c r="S10" s="1"/>
-      <c r="T10" s="21" t="s">
+      <c r="T10" s="29" t="s">
         <v>0</v>
       </c>
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
       <c r="W10" s="9"/>
-      <c r="X10" s="21"/>
+      <c r="X10" s="29"/>
     </row>
     <row r="11" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21" t="s">
+      <c r="A11" s="29" t="s">
         <v>56</v>
       </c>
       <c r="B11" s="1" t="s">
@@ -1557,7 +1579,7 @@
       <c r="D11" s="9"/>
       <c r="E11" s="9"/>
       <c r="F11" s="9"/>
-      <c r="G11" s="21" t="s">
+      <c r="G11" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H11" s="9"/>
@@ -1572,48 +1594,50 @@
       <c r="Q11" s="9"/>
       <c r="R11" s="9"/>
       <c r="S11" s="9"/>
-      <c r="T11" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U11" s="1"/>
+      <c r="T11" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U11" s="16" t="s">
+        <v>103</v>
+      </c>
       <c r="V11" s="1"/>
       <c r="W11" s="9"/>
-      <c r="X11" s="21"/>
+      <c r="X11" s="29"/>
     </row>
     <row r="12" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
+      <c r="A12" s="29"/>
       <c r="B12" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F12" s="16"/>
-      <c r="G12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H12" s="13" t="s">
+      <c r="D12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F12" s="15"/>
+      <c r="G12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H12" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L12" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M12" s="13" t="s">
+      <c r="I12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L12" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M12" s="12" t="s">
         <v>63</v>
       </c>
       <c r="N12" s="9"/>
@@ -1622,18 +1646,18 @@
       <c r="Q12" s="9"/>
       <c r="R12" s="9"/>
       <c r="S12" s="9"/>
-      <c r="T12" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U12" s="1"/>
+      <c r="T12" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U12" s="17"/>
       <c r="V12" s="1"/>
       <c r="W12" s="9" t="s">
         <v>82</v>
       </c>
-      <c r="X12" s="21"/>
+      <c r="X12" s="29"/>
     </row>
     <row r="13" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21"/>
+      <c r="A13" s="29"/>
       <c r="B13" s="1" t="s">
         <v>52</v>
       </c>
@@ -1641,83 +1665,83 @@
       <c r="D13" s="9"/>
       <c r="E13" s="9"/>
       <c r="F13" s="9"/>
-      <c r="G13" s="21" t="s">
+      <c r="G13" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H13" s="9"/>
       <c r="I13" s="9"/>
       <c r="J13" s="9"/>
       <c r="K13" s="9"/>
-      <c r="L13" s="13" t="s">
+      <c r="L13" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="P13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="R13" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="S13" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="T13" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U13" s="1"/>
+      <c r="M13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="P13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="R13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="S13" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="T13" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U13" s="17"/>
       <c r="V13" s="1"/>
       <c r="W13" s="9" t="s">
         <v>76</v>
       </c>
-      <c r="X13" s="21"/>
+      <c r="X13" s="29"/>
     </row>
     <row r="14" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
+      <c r="A14" s="29"/>
       <c r="B14" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G14" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H14" s="13" t="s">
+      <c r="D14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G14" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H14" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L14" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M14" s="13" t="s">
+      <c r="I14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L14" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M14" s="12" t="s">
         <v>63</v>
       </c>
       <c r="N14" s="9"/>
@@ -1726,43 +1750,43 @@
       <c r="Q14" s="9"/>
       <c r="R14" s="9"/>
       <c r="S14" s="9"/>
-      <c r="T14" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U14" s="1"/>
+      <c r="T14" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U14" s="17"/>
       <c r="V14" s="1"/>
       <c r="W14" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X14" s="21"/>
+      <c r="X14" s="29"/>
     </row>
     <row r="15" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
+      <c r="A15" s="29"/>
       <c r="B15" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C15" s="9"/>
       <c r="D15" s="9"/>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="G15" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H15" s="23" t="s">
+      <c r="G15" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H15" s="19" t="s">
         <v>85</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="19" t="s">
         <v>86</v>
       </c>
-      <c r="J15" s="14"/>
-      <c r="K15" s="23" t="s">
+      <c r="J15" s="13"/>
+      <c r="K15" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="M15" s="19" t="s">
+      <c r="M15" s="32" t="s">
         <v>87</v>
       </c>
       <c r="N15" s="9"/>
@@ -1771,48 +1795,48 @@
       <c r="Q15" s="9"/>
       <c r="R15" s="9"/>
       <c r="S15" s="9"/>
-      <c r="T15" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U15" s="1"/>
+      <c r="T15" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U15" s="17"/>
       <c r="V15" s="1"/>
       <c r="W15" s="9"/>
-      <c r="X15" s="21"/>
+      <c r="X15" s="29"/>
     </row>
     <row r="16" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21"/>
+      <c r="A16" s="29"/>
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="9"/>
-      <c r="E16" s="18"/>
-      <c r="F16" s="18"/>
-      <c r="G16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H16" s="18"/>
-      <c r="I16" s="18"/>
-      <c r="J16" s="14"/>
-      <c r="K16" s="18"/>
-      <c r="L16" s="14"/>
-      <c r="M16" s="28"/>
+      <c r="E16" s="20"/>
+      <c r="F16" s="20"/>
+      <c r="G16" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20"/>
+      <c r="I16" s="20"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="20"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="26"/>
       <c r="N16" s="9"/>
       <c r="O16" s="9"/>
       <c r="P16" s="9"/>
       <c r="Q16" s="9"/>
       <c r="R16" s="9"/>
       <c r="S16" s="9"/>
-      <c r="T16" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="U16" s="1"/>
+      <c r="T16" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="U16" s="18"/>
       <c r="V16" s="1"/>
       <c r="W16" s="9"/>
-      <c r="X16" s="21"/>
+      <c r="X16" s="29"/>
     </row>
     <row r="17" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21" t="s">
+      <c r="A17" s="29" t="s">
         <v>57</v>
       </c>
       <c r="B17" s="1" t="s">
@@ -1822,16 +1846,16 @@
       <c r="D17" s="9"/>
       <c r="E17" s="9"/>
       <c r="F17" s="9"/>
-      <c r="G17" s="21" t="s">
+      <c r="G17" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H17" s="9"/>
       <c r="I17" s="9"/>
       <c r="J17" s="9"/>
-      <c r="K17" s="12" t="s">
+      <c r="K17" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="L17" s="12" t="s">
+      <c r="L17" s="11" t="s">
         <v>94</v>
       </c>
       <c r="M17" s="9"/>
@@ -1842,13 +1866,15 @@
       <c r="R17" s="9"/>
       <c r="S17" s="9"/>
       <c r="T17" s="1"/>
-      <c r="U17" s="1"/>
+      <c r="U17" s="16" t="s">
+        <v>104</v>
+      </c>
       <c r="V17" s="1"/>
       <c r="W17" s="9"/>
-      <c r="X17" s="21"/>
+      <c r="X17" s="29"/>
     </row>
     <row r="18" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
+      <c r="A18" s="29"/>
       <c r="B18" s="1" t="s">
         <v>51</v>
       </c>
@@ -1856,7 +1882,7 @@
       <c r="D18" s="9"/>
       <c r="E18" s="9"/>
       <c r="F18" s="9"/>
-      <c r="G18" s="21" t="s">
+      <c r="G18" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H18" s="9"/>
@@ -1872,13 +1898,13 @@
       <c r="R18" s="9"/>
       <c r="S18" s="9"/>
       <c r="T18" s="1"/>
-      <c r="U18" s="1"/>
+      <c r="U18" s="17"/>
       <c r="V18" s="1"/>
       <c r="W18" s="9"/>
-      <c r="X18" s="21"/>
+      <c r="X18" s="29"/>
     </row>
     <row r="19" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21"/>
+      <c r="A19" s="29"/>
       <c r="B19" s="1" t="s">
         <v>52</v>
       </c>
@@ -1886,45 +1912,45 @@
       <c r="D19" s="9"/>
       <c r="E19" s="9"/>
       <c r="F19" s="9"/>
-      <c r="G19" s="21" t="s">
+      <c r="G19" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H19" s="9"/>
       <c r="I19" s="9"/>
-      <c r="J19" s="33" t="s">
+      <c r="J19" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="K19" s="33" t="s">
+      <c r="K19" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="33" t="s">
+      <c r="L19" s="23" t="s">
         <v>91</v>
       </c>
       <c r="M19" s="9"/>
-      <c r="N19" s="33" t="s">
+      <c r="N19" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="O19" s="33" t="s">
+      <c r="O19" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="P19" s="33" t="s">
+      <c r="P19" s="23" t="s">
         <v>93</v>
       </c>
-      <c r="Q19" s="23" t="s">
-        <v>103</v>
-      </c>
-      <c r="R19" s="29" t="s">
-        <v>103</v>
+      <c r="Q19" s="19" t="s">
+        <v>102</v>
+      </c>
+      <c r="R19" s="19" t="s">
+        <v>102</v>
       </c>
       <c r="S19" s="9"/>
       <c r="T19" s="1"/>
-      <c r="U19" s="1"/>
+      <c r="U19" s="17"/>
       <c r="V19" s="1"/>
       <c r="W19" s="9"/>
-      <c r="X19" s="21"/>
+      <c r="X19" s="29"/>
     </row>
     <row r="20" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
+      <c r="A20" s="29"/>
       <c r="B20" s="1" t="s">
         <v>53</v>
       </c>
@@ -1932,29 +1958,29 @@
       <c r="D20" s="9"/>
       <c r="E20" s="9"/>
       <c r="F20" s="9"/>
-      <c r="G20" s="21" t="s">
+      <c r="G20" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H20" s="9"/>
       <c r="I20" s="9"/>
-      <c r="J20" s="34"/>
-      <c r="K20" s="34"/>
-      <c r="L20" s="34"/>
+      <c r="J20" s="24"/>
+      <c r="K20" s="24"/>
+      <c r="L20" s="24"/>
       <c r="M20" s="9"/>
-      <c r="N20" s="34"/>
-      <c r="O20" s="34"/>
-      <c r="P20" s="34"/>
-      <c r="Q20" s="24"/>
-      <c r="R20" s="30"/>
+      <c r="N20" s="24"/>
+      <c r="O20" s="24"/>
+      <c r="P20" s="24"/>
+      <c r="Q20" s="27"/>
+      <c r="R20" s="27"/>
       <c r="S20" s="9"/>
       <c r="T20" s="1"/>
-      <c r="U20" s="1"/>
+      <c r="U20" s="17"/>
       <c r="V20" s="1"/>
       <c r="W20" s="9"/>
-      <c r="X20" s="21"/>
+      <c r="X20" s="29"/>
     </row>
     <row r="21" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="1" t="s">
         <v>54</v>
       </c>
@@ -1962,16 +1988,16 @@
       <c r="D21" s="9"/>
       <c r="E21" s="9"/>
       <c r="F21" s="9"/>
-      <c r="G21" s="21" t="s">
+      <c r="G21" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H21" s="9"/>
       <c r="I21" s="9"/>
       <c r="J21" s="9"/>
-      <c r="K21" s="12" t="s">
+      <c r="K21" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="L21" s="12" t="s">
+      <c r="L21" s="11" t="s">
         <v>96</v>
       </c>
       <c r="M21" s="9"/>
@@ -1982,13 +2008,13 @@
       <c r="R21" s="9"/>
       <c r="S21" s="9"/>
       <c r="T21" s="1"/>
-      <c r="U21" s="1"/>
+      <c r="U21" s="17"/>
       <c r="V21" s="1"/>
       <c r="W21" s="9"/>
-      <c r="X21" s="21"/>
+      <c r="X21" s="29"/>
     </row>
     <row r="22" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
+      <c r="A22" s="29"/>
       <c r="B22" s="1" t="s">
         <v>55</v>
       </c>
@@ -1996,7 +2022,7 @@
       <c r="D22" s="9"/>
       <c r="E22" s="9"/>
       <c r="F22" s="9"/>
-      <c r="G22" s="21" t="s">
+      <c r="G22" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H22" s="9"/>
@@ -2012,13 +2038,13 @@
       <c r="R22" s="9"/>
       <c r="S22" s="9"/>
       <c r="T22" s="1"/>
-      <c r="U22" s="1"/>
+      <c r="U22" s="18"/>
       <c r="V22" s="1"/>
       <c r="W22" s="9"/>
-      <c r="X22" s="21"/>
+      <c r="X22" s="29"/>
     </row>
     <row r="23" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21" t="s">
+      <c r="A23" s="29" t="s">
         <v>58</v>
       </c>
       <c r="B23" s="1" t="s">
@@ -2028,7 +2054,7 @@
       <c r="D23" s="9"/>
       <c r="E23" s="9"/>
       <c r="F23" s="9"/>
-      <c r="G23" s="21" t="s">
+      <c r="G23" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H23" s="9"/>
@@ -2044,13 +2070,15 @@
       <c r="R23" s="9"/>
       <c r="S23" s="9"/>
       <c r="T23" s="1"/>
-      <c r="U23" s="1"/>
+      <c r="U23" s="16" t="s">
+        <v>105</v>
+      </c>
       <c r="V23" s="1"/>
       <c r="W23" s="9"/>
-      <c r="X23" s="21"/>
+      <c r="X23" s="29"/>
     </row>
     <row r="24" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21"/>
+      <c r="A24" s="29"/>
       <c r="B24" s="1" t="s">
         <v>51</v>
       </c>
@@ -2058,7 +2086,7 @@
       <c r="D24" s="9"/>
       <c r="E24" s="9"/>
       <c r="F24" s="9"/>
-      <c r="G24" s="21" t="s">
+      <c r="G24" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H24" s="9"/>
@@ -2074,149 +2102,149 @@
       <c r="R24" s="9"/>
       <c r="S24" s="9"/>
       <c r="T24" s="10"/>
-      <c r="U24" s="1"/>
+      <c r="U24" s="17"/>
       <c r="V24" s="1"/>
       <c r="W24" s="9"/>
-      <c r="X24" s="21"/>
+      <c r="X24" s="29"/>
     </row>
     <row r="25" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
+      <c r="A25" s="29"/>
       <c r="B25" s="1" t="s">
         <v>52</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="D25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G25" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H25" s="13" t="s">
+      <c r="D25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G25" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H25" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="I25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L25" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M25" s="33" t="s">
+      <c r="I25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L25" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M25" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="N25" s="33" t="s">
+      <c r="N25" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="O25" s="33" t="s">
+      <c r="O25" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="P25" s="33" t="s">
+      <c r="P25" s="23" t="s">
         <v>93</v>
       </c>
       <c r="Q25" s="9"/>
       <c r="R25" s="9"/>
       <c r="S25" s="9"/>
       <c r="T25" s="1"/>
-      <c r="U25" s="1"/>
+      <c r="U25" s="17"/>
       <c r="V25" s="1"/>
       <c r="W25" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="X25" s="21"/>
+      <c r="X25" s="29"/>
     </row>
     <row r="26" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
+      <c r="A26" s="29"/>
       <c r="B26" s="1" t="s">
         <v>53</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="D26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="E26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="F26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G26" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H26" s="13" t="s">
+      <c r="D26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="E26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G26" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H26" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="I26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="L26" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="M26" s="34"/>
-      <c r="N26" s="34"/>
-      <c r="O26" s="34"/>
-      <c r="P26" s="34"/>
+      <c r="I26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L26" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="M26" s="24"/>
+      <c r="N26" s="24"/>
+      <c r="O26" s="24"/>
+      <c r="P26" s="24"/>
       <c r="Q26" s="9"/>
       <c r="R26" s="9"/>
       <c r="S26" s="9"/>
       <c r="T26" s="1"/>
-      <c r="U26" s="1"/>
+      <c r="U26" s="17"/>
       <c r="V26" s="1"/>
       <c r="W26" s="9" t="s">
         <v>83</v>
       </c>
-      <c r="X26" s="21"/>
+      <c r="X26" s="29"/>
     </row>
     <row r="27" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="21"/>
+      <c r="A27" s="29"/>
       <c r="B27" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C27" s="9"/>
       <c r="D27" s="9"/>
-      <c r="E27" s="17" t="s">
+      <c r="E27" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="17" t="s">
+      <c r="F27" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H27" s="17" t="s">
+      <c r="G27" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H27" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="I27" s="17" t="s">
+      <c r="I27" s="35" t="s">
         <v>89</v>
       </c>
       <c r="J27" s="9"/>
-      <c r="K27" s="19" t="s">
+      <c r="K27" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="L27" s="12" t="s">
+      <c r="L27" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="M27" s="35" t="s">
+      <c r="M27" s="25" t="s">
         <v>90</v>
       </c>
       <c r="N27" s="9"/>
@@ -2226,29 +2254,29 @@
       <c r="R27" s="9"/>
       <c r="S27" s="9"/>
       <c r="T27" s="1"/>
-      <c r="U27" s="1"/>
+      <c r="U27" s="17"/>
       <c r="V27" s="1"/>
       <c r="W27" s="9"/>
-      <c r="X27" s="21"/>
+      <c r="X27" s="29"/>
     </row>
     <row r="28" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="21"/>
+      <c r="A28" s="29"/>
       <c r="B28" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C28" s="9"/>
       <c r="D28" s="9"/>
-      <c r="E28" s="18"/>
-      <c r="F28" s="18"/>
-      <c r="G28" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H28" s="18"/>
-      <c r="I28" s="18"/>
+      <c r="E28" s="20"/>
+      <c r="F28" s="20"/>
+      <c r="G28" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H28" s="20"/>
+      <c r="I28" s="20"/>
       <c r="J28" s="9"/>
-      <c r="K28" s="18"/>
-      <c r="L28" s="15"/>
-      <c r="M28" s="28"/>
+      <c r="K28" s="20"/>
+      <c r="L28" s="14"/>
+      <c r="M28" s="26"/>
       <c r="N28" s="9"/>
       <c r="O28" s="9"/>
       <c r="P28" s="9"/>
@@ -2256,13 +2284,13 @@
       <c r="R28" s="9"/>
       <c r="S28" s="9"/>
       <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
+      <c r="U28" s="18"/>
       <c r="V28" s="1"/>
       <c r="W28" s="9"/>
-      <c r="X28" s="21"/>
+      <c r="X28" s="29"/>
     </row>
     <row r="29" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="21" t="s">
+      <c r="A29" s="29" t="s">
         <v>59</v>
       </c>
       <c r="B29" s="1" t="s">
@@ -2271,16 +2299,16 @@
       <c r="C29" s="9"/>
       <c r="D29" s="9"/>
       <c r="E29" s="9"/>
-      <c r="F29" s="13" t="s">
+      <c r="F29" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="G29" s="21" t="s">
+      <c r="G29" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H29" s="9"/>
       <c r="I29" s="9"/>
       <c r="J29" s="9"/>
-      <c r="K29" s="12" t="s">
+      <c r="K29" s="11" t="s">
         <v>95</v>
       </c>
       <c r="L29" s="9"/>
@@ -2295,45 +2323,45 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
       <c r="W29" s="9"/>
-      <c r="X29" s="21"/>
+      <c r="X29" s="29"/>
     </row>
     <row r="30" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21"/>
+      <c r="A30" s="29"/>
       <c r="B30" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C30" s="9"/>
       <c r="D30" s="9"/>
       <c r="E30" s="9"/>
-      <c r="G30" s="21" t="s">
+      <c r="G30" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H30" s="9"/>
       <c r="I30" s="9"/>
       <c r="J30" s="9"/>
       <c r="K30" s="9"/>
-      <c r="L30" s="13" t="s">
+      <c r="L30" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="M30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="N30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="O30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="P30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q30" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="R30" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="S30" s="11" t="s">
+      <c r="M30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="N30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="O30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="P30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="R30" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="S30" s="12" t="s">
         <v>63</v>
       </c>
       <c r="T30" s="1"/>
@@ -2342,42 +2370,42 @@
       <c r="W30" s="9" t="s">
         <v>84</v>
       </c>
-      <c r="X30" s="21"/>
+      <c r="X30" s="29"/>
     </row>
     <row r="31" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
+      <c r="A31" s="29"/>
       <c r="B31" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C31" s="9"/>
       <c r="D31" s="9"/>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="F31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="G31" s="21" t="s">
-        <v>0</v>
-      </c>
-      <c r="H31" s="13" t="s">
+      <c r="F31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="G31" s="29" t="s">
+        <v>0</v>
+      </c>
+      <c r="H31" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="I31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="J31" s="13" t="s">
-        <v>63</v>
-      </c>
-      <c r="K31" s="13" t="s">
+      <c r="I31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="J31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="K31" s="12" t="s">
         <v>63</v>
       </c>
       <c r="L31" s="9"/>
       <c r="M31" s="9"/>
-      <c r="N31" s="33" t="s">
+      <c r="N31" s="23" t="s">
         <v>91</v>
       </c>
-      <c r="O31" s="33" t="s">
+      <c r="O31" s="23" t="s">
         <v>93</v>
       </c>
       <c r="P31" s="9"/>
@@ -2390,10 +2418,10 @@
       <c r="W31" s="9" t="s">
         <v>75</v>
       </c>
-      <c r="X31" s="21"/>
+      <c r="X31" s="29"/>
     </row>
     <row r="32" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
+      <c r="A32" s="29"/>
       <c r="B32" s="1" t="s">
         <v>53</v>
       </c>
@@ -2401,7 +2429,7 @@
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
       <c r="F32" s="1"/>
-      <c r="G32" s="21" t="s">
+      <c r="G32" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H32" s="1"/>
@@ -2409,23 +2437,25 @@
       <c r="J32" s="1"/>
       <c r="K32" s="1"/>
       <c r="L32" s="1"/>
-      <c r="M32" s="12" t="s">
+      <c r="M32" s="11" t="s">
         <v>101</v>
       </c>
-      <c r="N32" s="34"/>
-      <c r="O32" s="34"/>
+      <c r="N32" s="24"/>
+      <c r="O32" s="24"/>
       <c r="P32" s="1"/>
       <c r="Q32" s="1"/>
       <c r="R32" s="1"/>
       <c r="S32" s="1"/>
-      <c r="T32" s="1"/>
+      <c r="T32" s="36" t="s">
+        <v>107</v>
+      </c>
       <c r="U32" s="1"/>
       <c r="V32" s="1"/>
       <c r="W32" s="1"/>
-      <c r="X32" s="21"/>
+      <c r="X32" s="29"/>
     </row>
     <row r="33" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21"/>
+      <c r="A33" s="29"/>
       <c r="B33" s="1" t="s">
         <v>54</v>
       </c>
@@ -2433,7 +2463,7 @@
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
       <c r="F33" s="1"/>
-      <c r="G33" s="21" t="s">
+      <c r="G33" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H33" s="1"/>
@@ -2443,7 +2473,7 @@
       <c r="L33" s="1"/>
       <c r="M33" s="1"/>
       <c r="N33" s="1"/>
-      <c r="O33" s="12" t="s">
+      <c r="O33" s="11" t="s">
         <v>101</v>
       </c>
       <c r="P33" s="1"/>
@@ -2454,10 +2484,10 @@
       <c r="U33" s="1"/>
       <c r="V33" s="1"/>
       <c r="W33" s="1"/>
-      <c r="X33" s="21"/>
+      <c r="X33" s="29"/>
     </row>
     <row r="34" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
+      <c r="A34" s="29"/>
       <c r="B34" s="1" t="s">
         <v>55</v>
       </c>
@@ -2465,7 +2495,7 @@
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
       <c r="F34" s="1"/>
-      <c r="G34" s="21" t="s">
+      <c r="G34" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H34" s="1"/>
@@ -2484,10 +2514,10 @@
       <c r="U34" s="1"/>
       <c r="V34" s="1"/>
       <c r="W34" s="1"/>
-      <c r="X34" s="21"/>
+      <c r="X34" s="29"/>
     </row>
     <row r="35" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21" t="s">
+      <c r="A35" s="29" t="s">
         <v>60</v>
       </c>
       <c r="B35" s="1" t="s">
@@ -2495,16 +2525,16 @@
       </c>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
-      <c r="E35" s="21" t="s">
+      <c r="E35" s="29" t="s">
         <v>70</v>
       </c>
       <c r="F35" s="1"/>
-      <c r="G35" s="21" t="s">
+      <c r="G35" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H35" s="1"/>
       <c r="I35" s="1"/>
-      <c r="J35" s="21" t="s">
+      <c r="J35" s="29" t="s">
         <v>68</v>
       </c>
       <c r="K35" s="1"/>
@@ -2513,7 +2543,7 @@
       <c r="N35" s="1"/>
       <c r="O35" s="1"/>
       <c r="P35" s="1"/>
-      <c r="Q35" s="23" t="s">
+      <c r="Q35" s="19" t="s">
         <v>99</v>
       </c>
       <c r="R35" s="1"/>
@@ -2522,25 +2552,25 @@
       <c r="U35" s="1"/>
       <c r="V35" s="1"/>
       <c r="W35" s="1"/>
-      <c r="X35" s="21"/>
+      <c r="X35" s="29"/>
     </row>
     <row r="36" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21"/>
+      <c r="A36" s="29"/>
       <c r="B36" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
-      <c r="E36" s="21" t="s">
+      <c r="E36" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F36" s="1"/>
-      <c r="G36" s="21" t="s">
+      <c r="G36" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H36" s="1"/>
       <c r="I36" s="1"/>
-      <c r="J36" s="21" t="s">
+      <c r="J36" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K36" s="1"/>
@@ -2549,32 +2579,32 @@
       <c r="N36" s="1"/>
       <c r="O36" s="1"/>
       <c r="P36" s="1"/>
-      <c r="Q36" s="18"/>
+      <c r="Q36" s="20"/>
       <c r="R36" s="1"/>
       <c r="S36" s="1"/>
       <c r="T36" s="1"/>
       <c r="U36" s="1"/>
       <c r="V36" s="1"/>
       <c r="W36" s="1"/>
-      <c r="X36" s="21"/>
+      <c r="X36" s="29"/>
     </row>
     <row r="37" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
+      <c r="A37" s="29"/>
       <c r="B37" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
-      <c r="E37" s="21" t="s">
+      <c r="E37" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F37" s="1"/>
-      <c r="G37" s="21" t="s">
+      <c r="G37" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H37" s="1"/>
       <c r="I37" s="1"/>
-      <c r="J37" s="21" t="s">
+      <c r="J37" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K37" s="1"/>
@@ -2590,25 +2620,25 @@
       <c r="U37" s="1"/>
       <c r="V37" s="1"/>
       <c r="W37" s="1"/>
-      <c r="X37" s="21"/>
+      <c r="X37" s="29"/>
     </row>
     <row r="38" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
+      <c r="A38" s="29"/>
       <c r="B38" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
-      <c r="E38" s="21" t="s">
+      <c r="E38" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F38" s="1"/>
-      <c r="G38" s="21" t="s">
+      <c r="G38" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H38" s="1"/>
       <c r="I38" s="1"/>
-      <c r="J38" s="21" t="s">
+      <c r="J38" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K38" s="1"/>
@@ -2624,25 +2654,25 @@
       <c r="U38" s="1"/>
       <c r="V38" s="1"/>
       <c r="W38" s="1"/>
-      <c r="X38" s="21"/>
+      <c r="X38" s="29"/>
     </row>
     <row r="39" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21"/>
+      <c r="A39" s="29"/>
       <c r="B39" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
-      <c r="E39" s="21" t="s">
+      <c r="E39" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F39" s="1"/>
-      <c r="G39" s="21" t="s">
+      <c r="G39" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H39" s="1"/>
       <c r="I39" s="1"/>
-      <c r="J39" s="21" t="s">
+      <c r="J39" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K39" s="1"/>
@@ -2658,25 +2688,25 @@
       <c r="U39" s="1"/>
       <c r="V39" s="1"/>
       <c r="W39" s="1"/>
-      <c r="X39" s="21"/>
+      <c r="X39" s="29"/>
     </row>
     <row r="40" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
+      <c r="A40" s="29"/>
       <c r="B40" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
-      <c r="E40" s="21" t="s">
+      <c r="E40" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F40" s="1"/>
-      <c r="G40" s="21" t="s">
+      <c r="G40" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H40" s="1"/>
       <c r="I40" s="1"/>
-      <c r="J40" s="21" t="s">
+      <c r="J40" s="29" t="s">
         <v>0</v>
       </c>
       <c r="K40" s="1"/>
@@ -2692,10 +2722,10 @@
       <c r="U40" s="1"/>
       <c r="V40" s="1"/>
       <c r="W40" s="1"/>
-      <c r="X40" s="21"/>
+      <c r="X40" s="29"/>
     </row>
     <row r="41" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21" t="s">
+      <c r="A41" s="29" t="s">
         <v>61</v>
       </c>
       <c r="B41" s="1" t="s">
@@ -2703,11 +2733,11 @@
       </c>
       <c r="C41" s="1"/>
       <c r="D41" s="1"/>
-      <c r="E41" s="21" t="s">
+      <c r="E41" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F41" s="1"/>
-      <c r="G41" s="21" t="s">
+      <c r="G41" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H41" s="1"/>
@@ -2721,7 +2751,7 @@
       <c r="P41" s="1"/>
       <c r="Q41" s="1"/>
       <c r="R41" s="1"/>
-      <c r="S41" s="21" t="s">
+      <c r="S41" s="29" t="s">
         <v>71</v>
       </c>
       <c r="T41" s="1"/>
@@ -2730,20 +2760,20 @@
       <c r="W41" s="4" t="s">
         <v>77</v>
       </c>
-      <c r="X41" s="21"/>
+      <c r="X41" s="29"/>
     </row>
     <row r="42" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
+      <c r="A42" s="29"/>
       <c r="B42" s="1" t="s">
         <v>51</v>
       </c>
       <c r="C42" s="1"/>
       <c r="D42" s="1"/>
-      <c r="E42" s="21" t="s">
+      <c r="E42" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F42" s="1"/>
-      <c r="G42" s="21" t="s">
+      <c r="G42" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H42" s="1"/>
@@ -2757,7 +2787,7 @@
       <c r="P42" s="1"/>
       <c r="Q42" s="1"/>
       <c r="R42" s="1"/>
-      <c r="S42" s="21" t="s">
+      <c r="S42" s="29" t="s">
         <v>0</v>
       </c>
       <c r="T42" s="1"/>
@@ -2766,20 +2796,20 @@
       <c r="W42" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="X42" s="21"/>
+      <c r="X42" s="29"/>
     </row>
     <row r="43" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="21"/>
+      <c r="A43" s="29"/>
       <c r="B43" s="1" t="s">
         <v>52</v>
       </c>
       <c r="C43" s="1"/>
       <c r="D43" s="1"/>
-      <c r="E43" s="21" t="s">
+      <c r="E43" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F43" s="1"/>
-      <c r="G43" s="21" t="s">
+      <c r="G43" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H43" s="1"/>
@@ -2793,7 +2823,7 @@
       <c r="P43" s="1"/>
       <c r="Q43" s="1"/>
       <c r="R43" s="1"/>
-      <c r="S43" s="21" t="s">
+      <c r="S43" s="29" t="s">
         <v>0</v>
       </c>
       <c r="T43" s="1"/>
@@ -2802,20 +2832,20 @@
       <c r="W43" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="X43" s="21"/>
+      <c r="X43" s="29"/>
     </row>
     <row r="44" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="1" t="s">
         <v>53</v>
       </c>
       <c r="C44" s="1"/>
       <c r="D44" s="1"/>
-      <c r="E44" s="21" t="s">
+      <c r="E44" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F44" s="1"/>
-      <c r="G44" s="21" t="s">
+      <c r="G44" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H44" s="1"/>
@@ -2829,7 +2859,7 @@
       <c r="P44" s="1"/>
       <c r="Q44" s="1"/>
       <c r="R44" s="1"/>
-      <c r="S44" s="21" t="s">
+      <c r="S44" s="29" t="s">
         <v>0</v>
       </c>
       <c r="T44" s="1"/>
@@ -2838,20 +2868,20 @@
       <c r="W44" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="X44" s="21"/>
+      <c r="X44" s="29"/>
     </row>
     <row r="45" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
+      <c r="A45" s="29"/>
       <c r="B45" s="1" t="s">
         <v>54</v>
       </c>
       <c r="C45" s="1"/>
       <c r="D45" s="1"/>
-      <c r="E45" s="21" t="s">
+      <c r="E45" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F45" s="1"/>
-      <c r="G45" s="21" t="s">
+      <c r="G45" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H45" s="1"/>
@@ -2865,7 +2895,7 @@
       <c r="P45" s="1"/>
       <c r="Q45" s="1"/>
       <c r="R45" s="1"/>
-      <c r="S45" s="21" t="s">
+      <c r="S45" s="29" t="s">
         <v>0</v>
       </c>
       <c r="T45" s="1"/>
@@ -2874,20 +2904,20 @@
       <c r="W45" s="8" t="s">
         <v>81</v>
       </c>
-      <c r="X45" s="21"/>
+      <c r="X45" s="29"/>
     </row>
     <row r="46" spans="1:24" ht="13.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
+      <c r="A46" s="29"/>
       <c r="B46" s="1" t="s">
         <v>55</v>
       </c>
       <c r="C46" s="1"/>
       <c r="D46" s="1"/>
-      <c r="E46" s="21" t="s">
+      <c r="E46" s="29" t="s">
         <v>0</v>
       </c>
       <c r="F46" s="1"/>
-      <c r="G46" s="21" t="s">
+      <c r="G46" s="29" t="s">
         <v>0</v>
       </c>
       <c r="H46" s="1"/>
@@ -2901,70 +2931,49 @@
       <c r="P46" s="1"/>
       <c r="Q46" s="1"/>
       <c r="R46" s="1"/>
-      <c r="S46" s="21" t="s">
+      <c r="S46" s="29" t="s">
         <v>0</v>
       </c>
       <c r="T46" s="1"/>
       <c r="U46" s="1"/>
       <c r="V46" s="1"/>
       <c r="W46" s="1"/>
-      <c r="X46" s="21"/>
+      <c r="X46" s="29"/>
     </row>
     <row r="47" spans="1:24" ht="32.1" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="20" t="s">
+      <c r="A47" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="B47" s="21"/>
-      <c r="C47" s="21"/>
-      <c r="D47" s="21"/>
-      <c r="E47" s="21"/>
-      <c r="F47" s="21"/>
-      <c r="G47" s="21"/>
-      <c r="H47" s="21"/>
-      <c r="I47" s="21"/>
-      <c r="J47" s="21"/>
-      <c r="K47" s="21"/>
-      <c r="L47" s="21"/>
-      <c r="M47" s="21"/>
-      <c r="N47" s="21"/>
-      <c r="O47" s="21"/>
-      <c r="P47" s="21"/>
-      <c r="Q47" s="21"/>
-      <c r="R47" s="21"/>
-      <c r="S47" s="21"/>
-      <c r="T47" s="21"/>
-      <c r="U47" s="21"/>
-      <c r="V47" s="21"/>
-      <c r="W47" s="21"/>
-      <c r="X47" s="21"/>
+      <c r="B47" s="29"/>
+      <c r="C47" s="29"/>
+      <c r="D47" s="29"/>
+      <c r="E47" s="29"/>
+      <c r="F47" s="29"/>
+      <c r="G47" s="29"/>
+      <c r="H47" s="29"/>
+      <c r="I47" s="29"/>
+      <c r="J47" s="29"/>
+      <c r="K47" s="29"/>
+      <c r="L47" s="29"/>
+      <c r="M47" s="29"/>
+      <c r="N47" s="29"/>
+      <c r="O47" s="29"/>
+      <c r="P47" s="29"/>
+      <c r="Q47" s="29"/>
+      <c r="R47" s="29"/>
+      <c r="S47" s="29"/>
+      <c r="T47" s="29"/>
+      <c r="U47" s="29"/>
+      <c r="V47" s="29"/>
+      <c r="W47" s="29"/>
+      <c r="X47" s="29"/>
     </row>
   </sheetData>
-  <mergeCells count="46">
-    <mergeCell ref="Q35:Q36"/>
-    <mergeCell ref="V7:V8"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="J19:J20"/>
-    <mergeCell ref="K19:K20"/>
-    <mergeCell ref="N31:N32"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="L19:L20"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N19:N20"/>
-    <mergeCell ref="M27:M28"/>
-    <mergeCell ref="O19:O20"/>
-    <mergeCell ref="O31:O32"/>
-    <mergeCell ref="P19:P20"/>
-    <mergeCell ref="P25:P26"/>
-    <mergeCell ref="Q19:Q20"/>
-    <mergeCell ref="A1:X1"/>
-    <mergeCell ref="A2:L2"/>
-    <mergeCell ref="M2:X2"/>
-    <mergeCell ref="A5:A10"/>
-    <mergeCell ref="A11:A16"/>
-    <mergeCell ref="I15:I16"/>
-    <mergeCell ref="K15:K16"/>
-    <mergeCell ref="M15:M16"/>
-    <mergeCell ref="R19:R20"/>
+  <mergeCells count="49">
+    <mergeCell ref="F27:F28"/>
+    <mergeCell ref="H27:H28"/>
+    <mergeCell ref="I27:I28"/>
+    <mergeCell ref="K27:K28"/>
     <mergeCell ref="A47:X47"/>
     <mergeCell ref="X5:X46"/>
     <mergeCell ref="J35:J40"/>
@@ -2980,12 +2989,36 @@
     <mergeCell ref="A41:A46"/>
     <mergeCell ref="E15:E16"/>
     <mergeCell ref="F15:F16"/>
+    <mergeCell ref="E27:E28"/>
+    <mergeCell ref="A1:X1"/>
+    <mergeCell ref="A2:L2"/>
+    <mergeCell ref="M2:X2"/>
+    <mergeCell ref="A5:A10"/>
+    <mergeCell ref="A11:A16"/>
+    <mergeCell ref="I15:I16"/>
+    <mergeCell ref="K15:K16"/>
+    <mergeCell ref="M15:M16"/>
     <mergeCell ref="H15:H16"/>
-    <mergeCell ref="E27:E28"/>
-    <mergeCell ref="F27:F28"/>
-    <mergeCell ref="H27:H28"/>
-    <mergeCell ref="I27:I28"/>
-    <mergeCell ref="K27:K28"/>
+    <mergeCell ref="U11:U16"/>
+    <mergeCell ref="J19:J20"/>
+    <mergeCell ref="K19:K20"/>
+    <mergeCell ref="N31:N32"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="L19:L20"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N19:N20"/>
+    <mergeCell ref="M27:M28"/>
+    <mergeCell ref="U17:U22"/>
+    <mergeCell ref="U23:U28"/>
+    <mergeCell ref="Q35:Q36"/>
+    <mergeCell ref="V7:V8"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="O19:O20"/>
+    <mergeCell ref="O31:O32"/>
+    <mergeCell ref="P19:P20"/>
+    <mergeCell ref="P25:P26"/>
+    <mergeCell ref="Q19:Q20"/>
+    <mergeCell ref="R19:R20"/>
   </mergeCells>
   <phoneticPr fontId="7" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>